<commit_message>
Update MCMC analysis: refactor code structure, add new analysis scripts, and update outputs (with LFS for large pickle files)
</commit_message>
<xml_diff>
--- a/outputs/excel/bivariate_estimation_summaries.xlsx
+++ b/outputs/excel/bivariate_estimation_summaries.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Table 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table 4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -37,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -51,15 +54,45 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -534,4 +567,1346 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Pareto/NBD</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>HB M1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>HB M2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Disaggregate measure</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Correlation (Validation)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Correlation (Calibration)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MSE (Validation)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MSE (Calibration)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Aggregate measure</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Time-series MAPE (%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MAPE (Validation)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>55.26</v>
+      </c>
+      <c r="C11" t="n">
+        <v>55.26</v>
+      </c>
+      <c r="D11" t="n">
+        <v>55.26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MAPE (Calibration)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>52.06</v>
+      </c>
+      <c r="C12" t="n">
+        <v>52.06</v>
+      </c>
+      <c r="D12" t="n">
+        <v>52.06</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MAPE (Pooled)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>55.25</v>
+      </c>
+      <c r="C13" t="n">
+        <v>55.25</v>
+      </c>
+      <c r="D13" t="n">
+        <v>55.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>HB M1 (no covariates)</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>HB M2 (with a covariate)</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="3" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>2.5%</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>97.5%</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>2.5%</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>97.5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Purchase rate log(λ) - Intercept</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-3.51</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-3.38</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-3.71</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-3.52</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-3.33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Purchase rate log(λ) - Initial amount ($ 10^-3)</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Dropout rate log(μ) - Intercept</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-4.36</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-3.73</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-3.24</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-4.04</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-3.66</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-3.34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Dropout rate log(μ) - Initial amount ($ 10^-3)</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>sigma^2_λ = var[log λ]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>sigma^2_μ = var[log μ]</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>sigma_λ_μ = cov[log λ, log μ]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6.66</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Correlation computed from Γ₀</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Marginal log-likelihood</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-14816</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-14958</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Mean(λ)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2.5% tile λ</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>97.5% tile λ</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mean(μ)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2.5% tile μ</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>97.5% tile μ</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Mean exp lifetime (yrs)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Survival rate (1yr)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>P(alive at T_cal)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Exp # of trans in val period</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.481</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.016</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0693</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>21.41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.994</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0559</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.988</v>
+      </c>
+      <c r="K3" t="n">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.742</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0143</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0566</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.302</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.799</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0179</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0828</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.994</v>
+      </c>
+      <c r="K5" t="n">
+        <v>14.26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.436</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.629</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0552</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.469</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="K6" t="n">
+        <v>12.64</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.389</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.636</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0159</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0573</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.437</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.981</v>
+      </c>
+      <c r="K7" t="n">
+        <v>11.08</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.217</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0152</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0607</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.453</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.956</v>
+      </c>
+      <c r="K8" t="n">
+        <v>10.97</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.555</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.07489999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>9.699999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.306</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.169</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.469</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0142</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0727</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.478</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.994</v>
+      </c>
+      <c r="K10" t="n">
+        <v>9.109999999999999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.169</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0602</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.969</v>
+      </c>
+      <c r="K11" t="n">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>…</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>2348</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0301</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.6112</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.209</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.262</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>2349</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0346</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.8828</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>2350</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.0986</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>2351</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0322</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0017</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.8973</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.187</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.206</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>2352</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.2325</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>2353</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0418</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.4593</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>2354</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.152</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.648</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0457</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.0194</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>2355</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.431</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.036</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0408</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.3681</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>2356</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2.277</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5.066</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0446</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.4433</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>2357</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.223</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.536</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0418</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.3839</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Ave</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.058</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0274</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.7522</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.257</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0385</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2.277</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5.877</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0457</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="G25" t="n">
+        <v>14.9756</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.5610000000000001</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>21.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update analysis with full dataset, exclude pickle files from tracking
</commit_message>
<xml_diff>
--- a/outputs/excel/bivariate_estimation_summaries.xlsx
+++ b/outputs/excel/bivariate_estimation_summaries.xlsx
@@ -621,7 +621,7 @@
         <v>0.58</v>
       </c>
       <c r="D3" t="n">
-        <v>0.57</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="4">
@@ -637,7 +637,7 @@
         <v>0.99</v>
       </c>
       <c r="D4" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="6">
@@ -650,10 +650,10 @@
         <v>2.57</v>
       </c>
       <c r="C6" t="n">
-        <v>2.97</v>
+        <v>2.98</v>
       </c>
       <c r="D6" t="n">
-        <v>3.05</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="7">
@@ -666,10 +666,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
       <c r="D7" t="n">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="9">
@@ -810,13 +810,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3.7</v>
+        <v>-3.73</v>
       </c>
       <c r="C4" t="n">
         <v>-3.51</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.38</v>
+        <v>-3.34</v>
       </c>
       <c r="E4" t="n">
         <v>-3.71</v>
@@ -825,7 +825,7 @@
         <v>-3.52</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.33</v>
+        <v>-3.34</v>
       </c>
     </row>
     <row r="5">
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F5" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="6">
@@ -851,22 +851,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-4.36</v>
+        <v>-4.21</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.73</v>
+        <v>-3.7</v>
       </c>
       <c r="D6" t="n">
-        <v>-3.24</v>
+        <v>-3.31</v>
       </c>
       <c r="E6" t="n">
         <v>-4.04</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.66</v>
+        <v>-3.65</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.34</v>
+        <v>-3.35</v>
       </c>
     </row>
     <row r="7">
@@ -876,13 +876,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.22</v>
+        <v>-0.3</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="G7" t="n">
-        <v>0.21</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8">
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.13</v>
+        <v>1.1</v>
       </c>
       <c r="C8" t="n">
-        <v>1.4</v>
+        <v>1.37</v>
       </c>
       <c r="D8" t="n">
-        <v>1.83</v>
+        <v>1.74</v>
       </c>
       <c r="E8" t="n">
-        <v>1.13</v>
+        <v>1.08</v>
       </c>
       <c r="F8" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="G8" t="n">
-        <v>1.58</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="9">
@@ -920,19 +920,19 @@
         <v>-0.14</v>
       </c>
       <c r="C9" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="D9" t="n">
-        <v>1.17</v>
+        <v>1.01</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.14</v>
+        <v>-0.18</v>
       </c>
       <c r="F9" t="n">
         <v>0.26</v>
       </c>
       <c r="G9" t="n">
-        <v>0.87</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="10">
@@ -942,22 +942,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.4</v>
+        <v>2.23</v>
       </c>
       <c r="C10" t="n">
-        <v>3.87</v>
+        <v>3.8</v>
       </c>
       <c r="D10" t="n">
-        <v>6.66</v>
+        <v>6.08</v>
       </c>
       <c r="E10" t="n">
-        <v>1.66</v>
+        <v>1.64</v>
       </c>
       <c r="F10" t="n">
         <v>3.29</v>
       </c>
       <c r="G10" t="n">
-        <v>5.45</v>
+        <v>5.66</v>
       </c>
     </row>
     <row r="11">
@@ -967,22 +967,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.06</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="C11" t="n">
         <v>0.15</v>
       </c>
       <c r="D11" t="n">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="G11" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="12">
@@ -992,10 +992,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-14816</v>
+        <v>-14845</v>
       </c>
       <c r="F12" t="n">
-        <v>-14958</v>
+        <v>-14943</v>
       </c>
     </row>
   </sheetData>
@@ -1083,34 +1083,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.751</v>
+        <v>0.756</v>
       </c>
       <c r="C2" t="n">
-        <v>0.481</v>
+        <v>0.489</v>
       </c>
       <c r="D2" t="n">
-        <v>1.016</v>
+        <v>1.076</v>
       </c>
       <c r="E2" t="n">
-        <v>0.017</v>
+        <v>0.016</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0008</v>
+        <v>0.0007</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0693</v>
+        <v>0.0701</v>
       </c>
       <c r="H2" t="n">
-        <v>1.13</v>
+        <v>1.2</v>
       </c>
       <c r="I2" t="n">
-        <v>0.413</v>
+        <v>0.435</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.998</v>
       </c>
       <c r="K2" t="n">
-        <v>21.41</v>
+        <v>21.88</v>
       </c>
     </row>
     <row r="3">
@@ -1118,34 +1118,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.715</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0.505</v>
+        <v>0.458</v>
       </c>
       <c r="D3" t="n">
-        <v>0.994</v>
+        <v>0.98</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0136</v>
+        <v>0.0143</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0009</v>
+        <v>0.0007</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0559</v>
+        <v>0.0605</v>
       </c>
       <c r="H3" t="n">
-        <v>1.42</v>
+        <v>1.34</v>
       </c>
       <c r="I3" t="n">
-        <v>0.494</v>
+        <v>0.475</v>
       </c>
       <c r="J3" t="n">
-        <v>0.988</v>
+        <v>0.996</v>
       </c>
       <c r="K3" t="n">
-        <v>21.39</v>
+        <v>20.63</v>
       </c>
     </row>
     <row r="4">
@@ -1153,34 +1153,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.504</v>
+        <v>0.514</v>
       </c>
       <c r="C4" t="n">
-        <v>0.305</v>
+        <v>0.294</v>
       </c>
       <c r="D4" t="n">
-        <v>0.742</v>
+        <v>0.794</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0143</v>
+        <v>0.0165</v>
       </c>
       <c r="F4" t="n">
-        <v>0.001</v>
+        <v>0.0007</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0566</v>
+        <v>0.07049999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>1.34</v>
+        <v>1.16</v>
       </c>
       <c r="I4" t="n">
-        <v>0.474</v>
+        <v>0.424</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>0.993</v>
       </c>
       <c r="K4" t="n">
-        <v>15.06</v>
+        <v>14.67</v>
       </c>
     </row>
     <row r="5">
@@ -1188,34 +1188,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.512</v>
+        <v>0.494</v>
       </c>
       <c r="C5" t="n">
-        <v>0.302</v>
+        <v>0.29</v>
       </c>
       <c r="D5" t="n">
-        <v>0.799</v>
+        <v>0.75</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0179</v>
+        <v>0.0148</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0013</v>
+        <v>0.0007</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0828</v>
+        <v>0.0636</v>
       </c>
       <c r="H5" t="n">
-        <v>1.07</v>
+        <v>1.3</v>
       </c>
       <c r="I5" t="n">
-        <v>0.393</v>
+        <v>0.464</v>
       </c>
       <c r="J5" t="n">
-        <v>0.994</v>
+        <v>0.998</v>
       </c>
       <c r="K5" t="n">
-        <v>14.26</v>
+        <v>14.63</v>
       </c>
     </row>
     <row r="6">
@@ -1223,34 +1223,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.436</v>
+        <v>0.446</v>
       </c>
       <c r="C6" t="n">
-        <v>0.251</v>
+        <v>0.261</v>
       </c>
       <c r="D6" t="n">
-        <v>0.629</v>
+        <v>0.681</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0146</v>
+        <v>0.0147</v>
       </c>
       <c r="F6" t="n">
         <v>0.0005999999999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0552</v>
+        <v>0.0622</v>
       </c>
       <c r="H6" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="I6" t="n">
-        <v>0.469</v>
+        <v>0.466</v>
       </c>
       <c r="J6" t="n">
-        <v>0.975</v>
+        <v>0.987</v>
       </c>
       <c r="K6" t="n">
-        <v>12.64</v>
+        <v>13.07</v>
       </c>
     </row>
     <row r="7">
@@ -1258,34 +1258,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.389</v>
+        <v>0.392</v>
       </c>
       <c r="C7" t="n">
-        <v>0.204</v>
+        <v>0.208</v>
       </c>
       <c r="D7" t="n">
-        <v>0.636</v>
+        <v>0.631</v>
       </c>
       <c r="E7" t="n">
         <v>0.0159</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0005</v>
+        <v>0.0007</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0573</v>
+        <v>0.0709</v>
       </c>
       <c r="H7" t="n">
         <v>1.21</v>
       </c>
       <c r="I7" t="n">
-        <v>0.437</v>
+        <v>0.438</v>
       </c>
       <c r="J7" t="n">
-        <v>0.981</v>
+        <v>0.98</v>
       </c>
       <c r="K7" t="n">
-        <v>11.08</v>
+        <v>11.15</v>
       </c>
     </row>
     <row r="8">
@@ -1293,34 +1293,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.39</v>
+        <v>0.378</v>
       </c>
       <c r="C8" t="n">
-        <v>0.217</v>
+        <v>0.195</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0152</v>
+        <v>0.0154</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0005</v>
+        <v>0.0007</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0607</v>
+        <v>0.0659</v>
       </c>
       <c r="H8" t="n">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
       <c r="I8" t="n">
-        <v>0.453</v>
+        <v>0.449</v>
       </c>
       <c r="J8" t="n">
-        <v>0.956</v>
+        <v>0.973</v>
       </c>
       <c r="K8" t="n">
-        <v>10.97</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="9">
@@ -1328,34 +1328,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.329</v>
+        <v>0.325</v>
       </c>
       <c r="C9" t="n">
         <v>0.174</v>
       </c>
       <c r="D9" t="n">
-        <v>0.555</v>
+        <v>0.537</v>
       </c>
       <c r="E9" t="n">
-        <v>0.015</v>
+        <v>0.0147</v>
       </c>
       <c r="F9" t="n">
-        <v>0.001</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>0.07489999999999999</v>
+        <v>0.063</v>
       </c>
       <c r="H9" t="n">
-        <v>1.28</v>
+        <v>1.3</v>
       </c>
       <c r="I9" t="n">
-        <v>0.458</v>
+        <v>0.464</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0.993</v>
       </c>
       <c r="K9" t="n">
-        <v>9.699999999999999</v>
+        <v>9.58</v>
       </c>
     </row>
     <row r="10">
@@ -1363,34 +1363,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.306</v>
+        <v>0.315</v>
       </c>
       <c r="C10" t="n">
-        <v>0.169</v>
+        <v>0.161</v>
       </c>
       <c r="D10" t="n">
-        <v>0.469</v>
+        <v>0.52</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0142</v>
+        <v>0.0147</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0009</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0727</v>
+        <v>0.0633</v>
       </c>
       <c r="H10" t="n">
-        <v>1.36</v>
+        <v>1.31</v>
       </c>
       <c r="I10" t="n">
-        <v>0.478</v>
+        <v>0.466</v>
       </c>
       <c r="J10" t="n">
-        <v>0.994</v>
+        <v>0.99</v>
       </c>
       <c r="K10" t="n">
-        <v>9.109999999999999</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="11">
@@ -1398,34 +1398,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.316</v>
+        <v>0.303</v>
       </c>
       <c r="C11" t="n">
-        <v>0.169</v>
+        <v>0.149</v>
       </c>
       <c r="D11" t="n">
-        <v>0.512</v>
+        <v>0.509</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0169</v>
+        <v>0.015</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0008</v>
+        <v>0.0007</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0602</v>
+        <v>0.0649</v>
       </c>
       <c r="H11" t="n">
-        <v>1.14</v>
+        <v>1.28</v>
       </c>
       <c r="I11" t="n">
-        <v>0.416</v>
+        <v>0.457</v>
       </c>
       <c r="J11" t="n">
-        <v>0.969</v>
+        <v>0.982</v>
       </c>
       <c r="K11" t="n">
-        <v>8.76</v>
+        <v>8.789999999999999</v>
       </c>
     </row>
     <row r="12">
@@ -1450,34 +1450,34 @@
         <v>2348</v>
       </c>
       <c r="B13" t="n">
-        <v>0.023</v>
+        <v>0.03</v>
       </c>
       <c r="C13" t="n">
         <v>0.002</v>
       </c>
       <c r="D13" t="n">
-        <v>0.083</v>
+        <v>0.142</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0301</v>
+        <v>0.0318</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0011</v>
+        <v>0.0009</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6112</v>
+        <v>1.1556</v>
       </c>
       <c r="H13" t="n">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="I13" t="n">
-        <v>0.209</v>
+        <v>0.192</v>
       </c>
       <c r="J13" t="n">
-        <v>0.262</v>
+        <v>0.282</v>
       </c>
       <c r="K13" t="n">
-        <v>0.14</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="14">
@@ -1485,34 +1485,34 @@
         <v>2349</v>
       </c>
       <c r="B14" t="n">
-        <v>0.025</v>
+        <v>0.031</v>
       </c>
       <c r="C14" t="n">
         <v>0.002</v>
       </c>
       <c r="D14" t="n">
-        <v>0.082</v>
+        <v>0.14</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0346</v>
+        <v>0.032</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0016</v>
+        <v>0.001</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8828</v>
+        <v>1.2876</v>
       </c>
       <c r="H14" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="I14" t="n">
-        <v>0.165</v>
+        <v>0.19</v>
       </c>
       <c r="J14" t="n">
-        <v>0.25</v>
+        <v>0.277</v>
       </c>
       <c r="K14" t="n">
-        <v>0.14</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="15">
@@ -1520,34 +1520,34 @@
         <v>2350</v>
       </c>
       <c r="B15" t="n">
-        <v>0.029</v>
+        <v>0.504</v>
       </c>
       <c r="C15" t="n">
-        <v>0.002</v>
+        <v>0.199</v>
       </c>
       <c r="D15" t="n">
-        <v>0.126</v>
+        <v>0.962</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0338</v>
+        <v>0.0372</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0015</v>
+        <v>0.0048</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0986</v>
+        <v>0.235</v>
       </c>
       <c r="H15" t="n">
-        <v>0.57</v>
+        <v>0.52</v>
       </c>
       <c r="I15" t="n">
-        <v>0.172</v>
+        <v>0.144</v>
       </c>
       <c r="J15" t="n">
-        <v>0.2</v>
+        <v>0.016</v>
       </c>
       <c r="K15" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="16">
@@ -1555,34 +1555,34 @@
         <v>2351</v>
       </c>
       <c r="B16" t="n">
-        <v>0.027</v>
+        <v>0.466</v>
       </c>
       <c r="C16" t="n">
-        <v>0.002</v>
+        <v>0.055</v>
       </c>
       <c r="D16" t="n">
-        <v>0.092</v>
+        <v>1.547</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0322</v>
+        <v>0.0441</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0017</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8973</v>
+        <v>0.9296</v>
       </c>
       <c r="H16" t="n">
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
       <c r="I16" t="n">
-        <v>0.187</v>
+        <v>0.101</v>
       </c>
       <c r="J16" t="n">
-        <v>0.206</v>
+        <v>0.018</v>
       </c>
       <c r="K16" t="n">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="17">
@@ -1590,34 +1590,34 @@
         <v>2352</v>
       </c>
       <c r="B17" t="n">
-        <v>0.287</v>
+        <v>0.371</v>
       </c>
       <c r="C17" t="n">
-        <v>0.075</v>
+        <v>0.093</v>
       </c>
       <c r="D17" t="n">
-        <v>0.77</v>
+        <v>0.87</v>
       </c>
       <c r="E17" t="n">
-        <v>0.038</v>
+        <v>0.0403</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0045</v>
+        <v>0.0064</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2325</v>
+        <v>0.3328</v>
       </c>
       <c r="H17" t="n">
-        <v>0.51</v>
+        <v>0.48</v>
       </c>
       <c r="I17" t="n">
-        <v>0.139</v>
+        <v>0.123</v>
       </c>
       <c r="J17" t="n">
-        <v>0.019</v>
+        <v>0.012</v>
       </c>
       <c r="K17" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="18">
@@ -1625,34 +1625,34 @@
         <v>2353</v>
       </c>
       <c r="B18" t="n">
-        <v>0.362</v>
+        <v>0.392</v>
       </c>
       <c r="C18" t="n">
-        <v>0.095</v>
+        <v>0.079</v>
       </c>
       <c r="D18" t="n">
-        <v>0.835</v>
+        <v>1.014</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0418</v>
+        <v>0.0422</v>
       </c>
       <c r="F18" t="n">
-        <v>0.006</v>
+        <v>0.0075</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4593</v>
+        <v>0.482</v>
       </c>
       <c r="H18" t="n">
         <v>0.46</v>
       </c>
       <c r="I18" t="n">
-        <v>0.114</v>
+        <v>0.112</v>
       </c>
       <c r="J18" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="K18" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="19">
@@ -1660,34 +1660,34 @@
         <v>2354</v>
       </c>
       <c r="B19" t="n">
-        <v>0.86</v>
+        <v>0.439</v>
       </c>
       <c r="C19" t="n">
-        <v>0.152</v>
+        <v>0.102</v>
       </c>
       <c r="D19" t="n">
-        <v>2.648</v>
+        <v>1.088</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0457</v>
+        <v>0.0413</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0165</v>
+        <v>0.0067</v>
       </c>
       <c r="G19" t="n">
-        <v>1.0194</v>
+        <v>0.4223</v>
       </c>
       <c r="H19" t="n">
-        <v>0.42</v>
+        <v>0.47</v>
       </c>
       <c r="I19" t="n">
-        <v>0.093</v>
+        <v>0.117</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="20">
@@ -1695,34 +1695,34 @@
         <v>2355</v>
       </c>
       <c r="B20" t="n">
-        <v>0.431</v>
+        <v>0.896</v>
       </c>
       <c r="C20" t="n">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="D20" t="n">
-        <v>1.036</v>
+        <v>2.613</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0408</v>
+        <v>0.0456</v>
       </c>
       <c r="F20" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.0112</v>
       </c>
       <c r="G20" t="n">
-        <v>0.3681</v>
+        <v>1.1252</v>
       </c>
       <c r="H20" t="n">
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="I20" t="n">
-        <v>0.12</v>
+        <v>0.093</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21">
@@ -1730,34 +1730,34 @@
         <v>2356</v>
       </c>
       <c r="B21" t="n">
-        <v>3.58</v>
+        <v>0.713</v>
       </c>
       <c r="C21" t="n">
-        <v>2.277</v>
+        <v>0.232</v>
       </c>
       <c r="D21" t="n">
-        <v>5.066</v>
+        <v>1.483</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0446</v>
+        <v>0.0427</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0145</v>
+        <v>0.0081</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4433</v>
+        <v>0.4105</v>
       </c>
       <c r="H21" t="n">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="I21" t="n">
-        <v>0.099</v>
+        <v>0.108</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22">
@@ -1765,28 +1765,28 @@
         <v>2357</v>
       </c>
       <c r="B22" t="n">
-        <v>0.751</v>
+        <v>3.526</v>
       </c>
       <c r="C22" t="n">
-        <v>0.223</v>
+        <v>2.07</v>
       </c>
       <c r="D22" t="n">
-        <v>1.536</v>
+        <v>5.364</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0418</v>
+        <v>0.0447</v>
       </c>
       <c r="F22" t="n">
-        <v>0.008</v>
+        <v>0.0104</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3839</v>
+        <v>0.5833</v>
       </c>
       <c r="H22" t="n">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="I22" t="n">
-        <v>0.114</v>
+        <v>0.098</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1802,31 +1802,31 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
       <c r="C23" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="D23" t="n">
-        <v>0.195</v>
+        <v>0.202</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0274</v>
+        <v>0.0275</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0011</v>
+        <v>0.0009</v>
       </c>
       <c r="G23" t="n">
-        <v>0.7522</v>
+        <v>0.8064</v>
       </c>
       <c r="H23" t="n">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="I23" t="n">
-        <v>0.257</v>
+        <v>0.256</v>
       </c>
       <c r="J23" t="n">
-        <v>0.446</v>
+        <v>0.443</v>
       </c>
       <c r="K23" t="n">
         <v>0.73</v>
@@ -1839,22 +1839,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.02</v>
+        <v>0.028</v>
       </c>
       <c r="C24" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="D24" t="n">
-        <v>0.063</v>
+        <v>0.083</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0111</v>
+        <v>0.0118</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0001</v>
+        <v>0.0003</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0385</v>
+        <v>0.0492</v>
       </c>
       <c r="H24" t="n">
         <v>0.42</v>
@@ -1876,34 +1876,34 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3.58</v>
+        <v>3.526</v>
       </c>
       <c r="C25" t="n">
-        <v>2.277</v>
+        <v>2.07</v>
       </c>
       <c r="D25" t="n">
-        <v>5.877</v>
+        <v>5.364</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0457</v>
+        <v>0.0456</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0165</v>
+        <v>0.0112</v>
       </c>
       <c r="G25" t="n">
-        <v>14.9756</v>
+        <v>11.7459</v>
       </c>
       <c r="H25" t="n">
-        <v>1.73</v>
+        <v>1.63</v>
       </c>
       <c r="I25" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.541</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>21.41</v>
+        <v>21.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update project: reorganize data processing, add new analyses and figures
</commit_message>
<xml_diff>
--- a/outputs/excel/bivariate_estimation_summaries.xlsx
+++ b/outputs/excel/bivariate_estimation_summaries.xlsx
@@ -618,10 +618,10 @@
         <v>0.63</v>
       </c>
       <c r="C3" t="n">
-        <v>0.58</v>
+        <v>0.57</v>
       </c>
       <c r="D3" t="n">
-        <v>0.58</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="4">
@@ -650,10 +650,10 @@
         <v>2.57</v>
       </c>
       <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
         <v>2.98</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.99</v>
       </c>
     </row>
     <row r="7">
@@ -666,10 +666,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="D7" t="n">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="9">
@@ -819,13 +819,13 @@
         <v>-3.34</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.71</v>
+        <v>-3.76</v>
       </c>
       <c r="F4" t="n">
-        <v>-3.52</v>
+        <v>-3.59</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.34</v>
+        <v>-3.41</v>
       </c>
     </row>
     <row r="5">
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="F5" t="n">
         <v>0.2</v>
       </c>
       <c r="G5" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6">
@@ -860,13 +860,13 @@
         <v>-3.31</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.04</v>
+        <v>-3.99</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.65</v>
+        <v>-3.62</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.35</v>
+        <v>-3.38</v>
       </c>
     </row>
     <row r="7">
@@ -876,13 +876,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.3</v>
+        <v>-0.22</v>
       </c>
       <c r="F7" t="n">
         <v>0.05</v>
       </c>
       <c r="G7" t="n">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="8">
@@ -901,13 +901,13 @@
         <v>1.74</v>
       </c>
       <c r="E8" t="n">
-        <v>1.08</v>
+        <v>1.11</v>
       </c>
       <c r="F8" t="n">
-        <v>1.33</v>
+        <v>1.36</v>
       </c>
       <c r="G8" t="n">
-        <v>1.6</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="9">
@@ -926,13 +926,13 @@
         <v>1.01</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.18</v>
+        <v>-0.19</v>
       </c>
       <c r="F9" t="n">
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.85</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="10">
@@ -951,13 +951,13 @@
         <v>6.08</v>
       </c>
       <c r="E10" t="n">
-        <v>1.64</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>3.29</v>
+        <v>1.82</v>
       </c>
       <c r="G10" t="n">
-        <v>5.66</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="11">
@@ -976,13 +976,13 @@
         <v>0.36</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.1</v>
+        <v>-0.13</v>
       </c>
       <c r="F11" t="n">
-        <v>0.13</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G11" t="n">
-        <v>0.33</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="12">
@@ -992,10 +992,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-14845</v>
+        <v>-14955</v>
       </c>
       <c r="F12" t="n">
-        <v>-14943</v>
+        <v>-14954</v>
       </c>
     </row>
   </sheetData>
@@ -1083,34 +1083,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.756</v>
+        <v>0.754</v>
       </c>
       <c r="C2" t="n">
-        <v>0.489</v>
+        <v>0.487</v>
       </c>
       <c r="D2" t="n">
-        <v>1.076</v>
+        <v>1.085</v>
       </c>
       <c r="E2" t="n">
-        <v>0.016</v>
+        <v>0.0161</v>
       </c>
       <c r="F2" t="n">
         <v>0.0007</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0701</v>
+        <v>0.0717</v>
       </c>
       <c r="H2" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="I2" t="n">
-        <v>0.435</v>
+        <v>0.433</v>
       </c>
       <c r="J2" t="n">
         <v>0.998</v>
       </c>
       <c r="K2" t="n">
-        <v>21.88</v>
+        <v>21.78</v>
       </c>
     </row>
     <row r="3">
@@ -1118,34 +1118,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.698</v>
       </c>
       <c r="C3" t="n">
-        <v>0.458</v>
+        <v>0.465</v>
       </c>
       <c r="D3" t="n">
-        <v>0.98</v>
+        <v>0.987</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0143</v>
+        <v>0.0145</v>
       </c>
       <c r="F3" t="n">
         <v>0.0007</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0605</v>
+        <v>0.0602</v>
       </c>
       <c r="H3" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="I3" t="n">
-        <v>0.475</v>
+        <v>0.471</v>
       </c>
       <c r="J3" t="n">
-        <v>0.996</v>
+        <v>0.995</v>
       </c>
       <c r="K3" t="n">
-        <v>20.63</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="4">
@@ -1153,34 +1153,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.514</v>
+        <v>0.513</v>
       </c>
       <c r="C4" t="n">
-        <v>0.294</v>
+        <v>0.29</v>
       </c>
       <c r="D4" t="n">
-        <v>0.794</v>
+        <v>0.793</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0165</v>
+        <v>0.0164</v>
       </c>
       <c r="F4" t="n">
         <v>0.0007</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07049999999999999</v>
+        <v>0.07190000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>1.16</v>
+        <v>1.17</v>
       </c>
       <c r="I4" t="n">
-        <v>0.424</v>
+        <v>0.425</v>
       </c>
       <c r="J4" t="n">
-        <v>0.993</v>
+        <v>0.992</v>
       </c>
       <c r="K4" t="n">
-        <v>14.67</v>
+        <v>14.66</v>
       </c>
     </row>
     <row r="5">
@@ -1188,34 +1188,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.494</v>
+        <v>0.493</v>
       </c>
       <c r="C5" t="n">
-        <v>0.29</v>
+        <v>0.293</v>
       </c>
       <c r="D5" t="n">
         <v>0.75</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0148</v>
+        <v>0.015</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0007</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0636</v>
+        <v>0.06270000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="I5" t="n">
-        <v>0.464</v>
+        <v>0.459</v>
       </c>
       <c r="J5" t="n">
         <v>0.998</v>
       </c>
       <c r="K5" t="n">
-        <v>14.63</v>
+        <v>14.54</v>
       </c>
     </row>
     <row r="6">
@@ -1226,31 +1226,31 @@
         <v>0.446</v>
       </c>
       <c r="C6" t="n">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
       <c r="D6" t="n">
-        <v>0.681</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0147</v>
+        <v>0.0148</v>
       </c>
       <c r="F6" t="n">
         <v>0.0005999999999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0622</v>
+        <v>0.0644</v>
       </c>
       <c r="H6" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="I6" t="n">
-        <v>0.466</v>
+        <v>0.462</v>
       </c>
       <c r="J6" t="n">
         <v>0.987</v>
       </c>
       <c r="K6" t="n">
-        <v>13.07</v>
+        <v>13.04</v>
       </c>
     </row>
     <row r="7">
@@ -1258,13 +1258,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.392</v>
+        <v>0.389</v>
       </c>
       <c r="C7" t="n">
-        <v>0.208</v>
+        <v>0.206</v>
       </c>
       <c r="D7" t="n">
-        <v>0.631</v>
+        <v>0.63</v>
       </c>
       <c r="E7" t="n">
         <v>0.0159</v>
@@ -1273,19 +1273,19 @@
         <v>0.0007</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0709</v>
+        <v>0.0712</v>
       </c>
       <c r="H7" t="n">
         <v>1.21</v>
       </c>
       <c r="I7" t="n">
-        <v>0.438</v>
+        <v>0.437</v>
       </c>
       <c r="J7" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="K7" t="n">
-        <v>11.15</v>
+        <v>11.07</v>
       </c>
     </row>
     <row r="8">
@@ -1296,31 +1296,31 @@
         <v>0.378</v>
       </c>
       <c r="C8" t="n">
-        <v>0.195</v>
+        <v>0.199</v>
       </c>
       <c r="D8" t="n">
-        <v>0.61</v>
+        <v>0.614</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0154</v>
+        <v>0.0158</v>
       </c>
       <c r="F8" t="n">
         <v>0.0007</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0659</v>
+        <v>0.0696</v>
       </c>
       <c r="H8" t="n">
-        <v>1.25</v>
+        <v>1.22</v>
       </c>
       <c r="I8" t="n">
-        <v>0.449</v>
+        <v>0.44</v>
       </c>
       <c r="J8" t="n">
-        <v>0.973</v>
+        <v>0.972</v>
       </c>
       <c r="K8" t="n">
-        <v>10.8</v>
+        <v>10.69</v>
       </c>
     </row>
     <row r="9">
@@ -1328,22 +1328,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.325</v>
+        <v>0.326</v>
       </c>
       <c r="C9" t="n">
-        <v>0.174</v>
+        <v>0.171</v>
       </c>
       <c r="D9" t="n">
-        <v>0.537</v>
+        <v>0.534</v>
       </c>
       <c r="E9" t="n">
         <v>0.0147</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0007</v>
       </c>
       <c r="G9" t="n">
-        <v>0.063</v>
+        <v>0.0622</v>
       </c>
       <c r="H9" t="n">
         <v>1.3</v>
@@ -1352,10 +1352,10 @@
         <v>0.464</v>
       </c>
       <c r="J9" t="n">
-        <v>0.993</v>
+        <v>0.994</v>
       </c>
       <c r="K9" t="n">
-        <v>9.58</v>
+        <v>9.609999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1363,34 +1363,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.315</v>
+        <v>0.318</v>
       </c>
       <c r="C10" t="n">
-        <v>0.161</v>
+        <v>0.162</v>
       </c>
       <c r="D10" t="n">
-        <v>0.52</v>
+        <v>0.523</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0147</v>
+        <v>0.0145</v>
       </c>
       <c r="F10" t="n">
         <v>0.0005999999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0633</v>
+        <v>0.0613</v>
       </c>
       <c r="H10" t="n">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
       <c r="I10" t="n">
-        <v>0.466</v>
+        <v>0.471</v>
       </c>
       <c r="J10" t="n">
-        <v>0.99</v>
+        <v>0.991</v>
       </c>
       <c r="K10" t="n">
-        <v>9.25</v>
+        <v>9.390000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -1398,34 +1398,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.303</v>
+        <v>0.292</v>
       </c>
       <c r="C11" t="n">
-        <v>0.149</v>
+        <v>0.151</v>
       </c>
       <c r="D11" t="n">
-        <v>0.509</v>
+        <v>0.479</v>
       </c>
       <c r="E11" t="n">
-        <v>0.015</v>
+        <v>0.0139</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0007</v>
+        <v>0.0005</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0649</v>
+        <v>0.057</v>
       </c>
       <c r="H11" t="n">
-        <v>1.28</v>
+        <v>1.38</v>
       </c>
       <c r="I11" t="n">
-        <v>0.457</v>
+        <v>0.485</v>
       </c>
       <c r="J11" t="n">
-        <v>0.982</v>
+        <v>0.998</v>
       </c>
       <c r="K11" t="n">
-        <v>8.789999999999999</v>
+        <v>8.77</v>
       </c>
     </row>
     <row r="12">
@@ -1450,7 +1450,7 @@
         <v>2348</v>
       </c>
       <c r="B13" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="C13" t="n">
         <v>0.002</v>
@@ -1459,22 +1459,22 @@
         <v>0.142</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0318</v>
+        <v>0.0317</v>
       </c>
       <c r="F13" t="n">
         <v>0.0009</v>
       </c>
       <c r="G13" t="n">
-        <v>1.1556</v>
+        <v>1.03</v>
       </c>
       <c r="H13" t="n">
         <v>0.61</v>
       </c>
       <c r="I13" t="n">
-        <v>0.192</v>
+        <v>0.193</v>
       </c>
       <c r="J13" t="n">
-        <v>0.282</v>
+        <v>0.281</v>
       </c>
       <c r="K13" t="n">
         <v>0.19</v>
@@ -1485,31 +1485,31 @@
         <v>2349</v>
       </c>
       <c r="B14" t="n">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="C14" t="n">
         <v>0.002</v>
       </c>
       <c r="D14" t="n">
-        <v>0.14</v>
+        <v>0.145</v>
       </c>
       <c r="E14" t="n">
-        <v>0.032</v>
+        <v>0.0317</v>
       </c>
       <c r="F14" t="n">
         <v>0.001</v>
       </c>
       <c r="G14" t="n">
-        <v>1.2876</v>
+        <v>1.1113</v>
       </c>
       <c r="H14" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="I14" t="n">
-        <v>0.19</v>
+        <v>0.192</v>
       </c>
       <c r="J14" t="n">
-        <v>0.277</v>
+        <v>0.285</v>
       </c>
       <c r="K14" t="n">
         <v>0.19</v>
@@ -1520,34 +1520,34 @@
         <v>2350</v>
       </c>
       <c r="B15" t="n">
-        <v>0.504</v>
+        <v>0.461</v>
       </c>
       <c r="C15" t="n">
-        <v>0.199</v>
+        <v>0.051</v>
       </c>
       <c r="D15" t="n">
-        <v>0.962</v>
+        <v>1.541</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0372</v>
+        <v>0.0439</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0048</v>
+        <v>0.0078</v>
       </c>
       <c r="G15" t="n">
-        <v>0.235</v>
+        <v>0.9691</v>
       </c>
       <c r="H15" t="n">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="I15" t="n">
-        <v>0.144</v>
+        <v>0.102</v>
       </c>
       <c r="J15" t="n">
-        <v>0.016</v>
+        <v>0.022</v>
       </c>
       <c r="K15" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="16">
@@ -1555,34 +1555,34 @@
         <v>2351</v>
       </c>
       <c r="B16" t="n">
-        <v>0.466</v>
+        <v>0.5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.055</v>
+        <v>0.195</v>
       </c>
       <c r="D16" t="n">
-        <v>1.547</v>
+        <v>0.955</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0441</v>
+        <v>0.0377</v>
       </c>
       <c r="F16" t="n">
-        <v>0.008399999999999999</v>
+        <v>0.0053</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9296</v>
+        <v>0.2275</v>
       </c>
       <c r="H16" t="n">
-        <v>0.44</v>
+        <v>0.51</v>
       </c>
       <c r="I16" t="n">
-        <v>0.101</v>
+        <v>0.141</v>
       </c>
       <c r="J16" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="K16" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="17">
@@ -1590,34 +1590,34 @@
         <v>2352</v>
       </c>
       <c r="B17" t="n">
-        <v>0.371</v>
+        <v>0.369</v>
       </c>
       <c r="C17" t="n">
-        <v>0.093</v>
+        <v>0.091</v>
       </c>
       <c r="D17" t="n">
-        <v>0.87</v>
+        <v>0.873</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0403</v>
+        <v>0.0399</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0064</v>
+        <v>0.0056</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3328</v>
+        <v>0.3355</v>
       </c>
       <c r="H17" t="n">
         <v>0.48</v>
       </c>
       <c r="I17" t="n">
-        <v>0.123</v>
+        <v>0.126</v>
       </c>
       <c r="J17" t="n">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="K17" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18">
@@ -1625,22 +1625,22 @@
         <v>2353</v>
       </c>
       <c r="B18" t="n">
-        <v>0.392</v>
+        <v>0.394</v>
       </c>
       <c r="C18" t="n">
-        <v>0.079</v>
+        <v>0.078</v>
       </c>
       <c r="D18" t="n">
-        <v>1.014</v>
+        <v>1.027</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0422</v>
+        <v>0.0421</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0075</v>
+        <v>0.0071</v>
       </c>
       <c r="G18" t="n">
-        <v>0.482</v>
+        <v>0.4646</v>
       </c>
       <c r="H18" t="n">
         <v>0.46</v>
@@ -1649,10 +1649,10 @@
         <v>0.112</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01</v>
+        <v>0.012</v>
       </c>
       <c r="K18" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="19">
@@ -1660,34 +1660,34 @@
         <v>2354</v>
       </c>
       <c r="B19" t="n">
-        <v>0.439</v>
+        <v>0.438</v>
       </c>
       <c r="C19" t="n">
         <v>0.102</v>
       </c>
       <c r="D19" t="n">
-        <v>1.088</v>
+        <v>1.07</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0413</v>
+        <v>0.0414</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0067</v>
+        <v>0.0069</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4223</v>
+        <v>0.4215</v>
       </c>
       <c r="H19" t="n">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="I19" t="n">
-        <v>0.117</v>
+        <v>0.116</v>
       </c>
       <c r="J19" t="n">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
       <c r="K19" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20">
@@ -1695,13 +1695,13 @@
         <v>2355</v>
       </c>
       <c r="B20" t="n">
-        <v>0.896</v>
+        <v>0.905</v>
       </c>
       <c r="C20" t="n">
-        <v>0.14</v>
+        <v>0.146</v>
       </c>
       <c r="D20" t="n">
-        <v>2.613</v>
+        <v>2.605</v>
       </c>
       <c r="E20" t="n">
         <v>0.0456</v>
@@ -1710,7 +1710,7 @@
         <v>0.0112</v>
       </c>
       <c r="G20" t="n">
-        <v>1.1252</v>
+        <v>1.2043</v>
       </c>
       <c r="H20" t="n">
         <v>0.42</v>
@@ -1733,28 +1733,28 @@
         <v>0.713</v>
       </c>
       <c r="C21" t="n">
-        <v>0.232</v>
+        <v>0.236</v>
       </c>
       <c r="D21" t="n">
-        <v>1.483</v>
+        <v>1.482</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0427</v>
+        <v>0.0425</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0081</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4105</v>
+        <v>0.4207</v>
       </c>
       <c r="H21" t="n">
         <v>0.45</v>
       </c>
       <c r="I21" t="n">
-        <v>0.108</v>
+        <v>0.11</v>
       </c>
       <c r="J21" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>0.01</v>
@@ -1765,22 +1765,22 @@
         <v>2357</v>
       </c>
       <c r="B22" t="n">
-        <v>3.526</v>
+        <v>3.547</v>
       </c>
       <c r="C22" t="n">
-        <v>2.07</v>
+        <v>2.066</v>
       </c>
       <c r="D22" t="n">
-        <v>5.364</v>
+        <v>5.34</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0447</v>
+        <v>0.0446</v>
       </c>
       <c r="F22" t="n">
         <v>0.0104</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5833</v>
+        <v>0.5867</v>
       </c>
       <c r="H22" t="n">
         <v>0.43</v>
@@ -1811,25 +1811,25 @@
         <v>0.202</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0275</v>
+        <v>0.0276</v>
       </c>
       <c r="F23" t="n">
         <v>0.0009</v>
       </c>
       <c r="G23" t="n">
-        <v>0.8064</v>
+        <v>0.7879</v>
       </c>
       <c r="H23" t="n">
         <v>0.76</v>
       </c>
       <c r="I23" t="n">
-        <v>0.256</v>
+        <v>0.255</v>
       </c>
       <c r="J23" t="n">
         <v>0.443</v>
       </c>
       <c r="K23" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="24">
@@ -1845,16 +1845,16 @@
         <v>0.002</v>
       </c>
       <c r="D24" t="n">
-        <v>0.083</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="E24" t="n">
         <v>0.0118</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0003</v>
+        <v>0.0004</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0492</v>
+        <v>0.0517</v>
       </c>
       <c r="H24" t="n">
         <v>0.42</v>
@@ -1876,13 +1876,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3.526</v>
+        <v>3.547</v>
       </c>
       <c r="C25" t="n">
-        <v>2.07</v>
+        <v>2.066</v>
       </c>
       <c r="D25" t="n">
-        <v>5.364</v>
+        <v>5.34</v>
       </c>
       <c r="E25" t="n">
         <v>0.0456</v>
@@ -1891,19 +1891,19 @@
         <v>0.0112</v>
       </c>
       <c r="G25" t="n">
-        <v>11.7459</v>
+        <v>14.8072</v>
       </c>
       <c r="H25" t="n">
-        <v>1.63</v>
+        <v>1.62</v>
       </c>
       <c r="I25" t="n">
-        <v>0.541</v>
+        <v>0.54</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>21.88</v>
+        <v>21.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>